<commit_message>
Added AddCandidatePO,excel operations and Test
</commit_message>
<xml_diff>
--- a/ScriptsDocs/JDdata.xlsx
+++ b/ScriptsDocs/JDdata.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756925D4-E81C-4C4D-B61E-74710EF039AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE6320C-84FB-4356-A6C8-DF44EEB6F42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JD" sheetId="1" r:id="rId1"/>
-    <sheet name="Candidate" sheetId="3" r:id="rId2"/>
+    <sheet name="Candidate" sheetId="4" r:id="rId2"/>
     <sheet name="Skills" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Client name</t>
   </si>
@@ -103,16 +103,69 @@
   </si>
   <si>
     <t>No Perks</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>contact_no</t>
+  </si>
+  <si>
+    <t>current_company</t>
+  </si>
+  <si>
+    <t>current_CTC</t>
+  </si>
+  <si>
+    <t>expected_CTC</t>
+  </si>
+  <si>
+    <t>Notice</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Test_can_aut01_FN</t>
+  </si>
+  <si>
+    <t>Test_can_aut01_LN</t>
+  </si>
+  <si>
+    <t>test@0001.gmail</t>
+  </si>
+  <si>
+    <t>Immediate</t>
+  </si>
+  <si>
+    <t>USD*</t>
+  </si>
+  <si>
+    <t>Infinite</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,16 +188,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -541,13 +597,81 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F450F1A-2162-44A6-9375-AAAFD1CB4FB6}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC8C7F8-5D4E-4222-BBF1-4F0209FF96CA}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2">
+        <v>943001022</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2">
+        <v>200000</v>
+      </c>
+      <c r="I2">
+        <v>300000</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{E18ABBB7-1060-4CFF-B76E-F22AB8374DA4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
resolved locator issues in addcandidate test
</commit_message>
<xml_diff>
--- a/ScriptsDocs/JDdata.xlsx
+++ b/ScriptsDocs/JDdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE6320C-84FB-4356-A6C8-DF44EEB6F42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43B07A6-5D72-45F2-9B39-880574BBA8C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Client name</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Infinite</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>USA</t>
   </si>
 </sst>
 </file>
@@ -598,19 +604,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC8C7F8-5D4E-4222-BBF1-4F0209FF96CA}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -638,8 +645,11 @@
       <c r="I1" t="s">
         <v>33</v>
       </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -650,7 +660,7 @@
         <v>38</v>
       </c>
       <c r="D2">
-        <v>943001022</v>
+        <v>123</v>
       </c>
       <c r="E2" t="s">
         <v>39</v>
@@ -666,6 +676,9 @@
       </c>
       <c r="I2">
         <v>300000</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding candidate with candidates
</commit_message>
<xml_diff>
--- a/ScriptsDocs/JDdata.xlsx
+++ b/ScriptsDocs/JDdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D508CD-1511-46D9-96A0-3B95BDEB4AF6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8024ECD4-6CF8-4A29-843B-357DE1EE4E29}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>